<commit_message>
update actions - relative direction
</commit_message>
<xml_diff>
--- a/src/attributions/attributions_ig_traj_100.xlsx
+++ b/src/attributions/attributions_ig_traj_100.xlsx
@@ -1576,13 +1576,13 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>-0</v>
@@ -1603,13 +1603,13 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
         <v>-0</v>
@@ -1630,13 +1630,13 @@
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="U3" t="n">
         <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
         <v>-0</v>
@@ -1657,13 +1657,13 @@
         <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AF3" t="n">
         <v>-0</v>
@@ -1684,13 +1684,13 @@
         <v>0</v>
       </c>
       <c r="AL3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AM3" t="n">
         <v>0</v>
       </c>
       <c r="AN3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AO3" t="n">
         <v>-0</v>
@@ -1711,13 +1711,13 @@
         <v>0</v>
       </c>
       <c r="AU3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AV3" t="n">
         <v>0</v>
       </c>
       <c r="AW3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AX3" t="n">
         <v>-0</v>
@@ -1738,13 +1738,13 @@
         <v>0</v>
       </c>
       <c r="BD3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BE3" t="n">
         <v>0</v>
       </c>
       <c r="BF3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BG3" t="n">
         <v>-0</v>
@@ -1765,13 +1765,13 @@
         <v>0</v>
       </c>
       <c r="BM3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BN3" t="n">
         <v>0</v>
       </c>
       <c r="BO3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BP3" t="n">
         <v>-0</v>
@@ -1792,13 +1792,13 @@
         <v>0</v>
       </c>
       <c r="BV3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BW3" t="n">
         <v>0</v>
       </c>
       <c r="BX3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BY3" t="n">
         <v>-0</v>
@@ -1819,13 +1819,13 @@
         <v>0</v>
       </c>
       <c r="CE3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CF3" t="n">
         <v>0</v>
       </c>
       <c r="CG3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CH3" t="n">
         <v>-0</v>
@@ -1846,13 +1846,13 @@
         <v>0</v>
       </c>
       <c r="CN3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CO3" t="n">
         <v>0</v>
       </c>
       <c r="CP3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CQ3" t="n">
         <v>-0</v>
@@ -1900,13 +1900,13 @@
         <v>0</v>
       </c>
       <c r="DF3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DG3" t="n">
         <v>0</v>
       </c>
       <c r="DH3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DI3" t="n">
         <v>-0</v>
@@ -1927,13 +1927,13 @@
         <v>0</v>
       </c>
       <c r="DO3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DP3" t="n">
         <v>0</v>
       </c>
       <c r="DQ3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DR3" t="n">
         <v>-0</v>
@@ -1981,13 +1981,13 @@
         <v>0</v>
       </c>
       <c r="EG3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EH3" t="n">
         <v>0</v>
       </c>
       <c r="EI3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EJ3" t="n">
         <v>-0</v>
@@ -2008,13 +2008,13 @@
         <v>0</v>
       </c>
       <c r="EP3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EQ3" t="n">
         <v>0</v>
       </c>
       <c r="ER3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="ES3" t="n">
         <v>-0</v>
@@ -2035,13 +2035,13 @@
         <v>0</v>
       </c>
       <c r="EY3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EZ3" t="n">
         <v>0</v>
       </c>
       <c r="FA3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FB3" t="n">
         <v>-0</v>
@@ -2062,13 +2062,13 @@
         <v>0</v>
       </c>
       <c r="FH3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FI3" t="n">
         <v>0</v>
       </c>
       <c r="FJ3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FK3" t="n">
         <v>-0</v>
@@ -2145,19 +2145,19 @@
         <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.2747017914699572</v>
+        <v>0.5528775001402585</v>
       </c>
       <c r="C4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3879568604994868</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.06206065321002414</v>
+        <v>-0.01453760429325892</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>-0.4667893949817093</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -2172,46 +2172,46 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.2501526499854858</v>
+        <v>0.417684068809007</v>
       </c>
       <c r="L4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.3769189989379249</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.0284888097311701</v>
+        <v>-0.02508747765506329</v>
       </c>
       <c r="O4" t="n">
-        <v>0</v>
+        <v>-0.5132373770722745</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="R4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
         <v>-0</v>
       </c>
       <c r="T4" t="n">
-        <v>-0.02778297597246213</v>
+        <v>0.08355225222456056</v>
       </c>
       <c r="U4" t="n">
         <v>-0</v>
       </c>
       <c r="V4" t="n">
-        <v>-0.05428506137782119</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>-0.2535920454087249</v>
+        <v>-0.01937822669010482</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>0.002658846508433222</v>
       </c>
       <c r="Y4" t="n">
         <v>-0</v>
@@ -2223,106 +2223,106 @@
         <v>0</v>
       </c>
       <c r="AB4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.08985015728225271</v>
+        <v>0.05032154152566831</v>
       </c>
       <c r="AD4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.114439273654505</v>
+        <v>-0</v>
       </c>
       <c r="AF4" t="n">
-        <v>-0.07711131991596037</v>
+        <v>0.0452238122739473</v>
       </c>
       <c r="AG4" t="n">
-        <v>-0</v>
+        <v>-0.0006138402386187273</v>
       </c>
       <c r="AH4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AI4" t="n">
         <v>-0</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AK4" t="n">
         <v>0</v>
       </c>
       <c r="AL4" t="n">
-        <v>-0.03346459145160705</v>
+        <v>0.04783611672034568</v>
       </c>
       <c r="AM4" t="n">
         <v>-0</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.0542904818228295</v>
+        <v>0</v>
       </c>
       <c r="AO4" t="n">
-        <v>-0.04260640946324355</v>
+        <v>0.01105260176864441</v>
       </c>
       <c r="AP4" t="n">
-        <v>-0</v>
+        <v>-0.09245244625987968</v>
       </c>
       <c r="AQ4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AR4" t="n">
         <v>-0</v>
       </c>
       <c r="AS4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AT4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AU4" t="n">
-        <v>-0.261976040419243</v>
+        <v>0.4422955460039922</v>
       </c>
       <c r="AV4" t="n">
         <v>-0</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.106284415769844</v>
+        <v>-0</v>
       </c>
       <c r="AX4" t="n">
-        <v>0.03873602986646049</v>
+        <v>0.02909958576290571</v>
       </c>
       <c r="AY4" t="n">
-        <v>0</v>
+        <v>-0.3422947096666415</v>
       </c>
       <c r="AZ4" t="n">
         <v>0</v>
       </c>
       <c r="BA4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BB4" t="n">
         <v>0</v>
       </c>
       <c r="BC4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BD4" t="n">
-        <v>-0.03759611586858531</v>
+        <v>0.1729184930104705</v>
       </c>
       <c r="BE4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.2473518844814027</v>
+        <v>0</v>
       </c>
       <c r="BG4" t="n">
-        <v>-0.0989177781941718</v>
+        <v>-0.1709748528180153</v>
       </c>
       <c r="BH4" t="n">
-        <v>-0</v>
+        <v>-0.205773175343103</v>
       </c>
       <c r="BI4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BJ4" t="n">
         <v>0</v>
@@ -2334,19 +2334,19 @@
         <v>-0</v>
       </c>
       <c r="BM4" t="n">
-        <v>0.0848823359938901</v>
+        <v>0.2002558661155981</v>
       </c>
       <c r="BN4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BO4" t="n">
-        <v>0.04188015412903629</v>
+        <v>-0</v>
       </c>
       <c r="BP4" t="n">
-        <v>-0.006163623004791758</v>
+        <v>0.1039353742559497</v>
       </c>
       <c r="BQ4" t="n">
-        <v>0</v>
+        <v>-0.002745880478777002</v>
       </c>
       <c r="BR4" t="n">
         <v>-0</v>
@@ -2358,28 +2358,28 @@
         <v>0</v>
       </c>
       <c r="BU4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BV4" t="n">
-        <v>-0.0738610003525489</v>
+        <v>0.2202303488753476</v>
       </c>
       <c r="BW4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BX4" t="n">
-        <v>0.1391207985656774</v>
+        <v>0</v>
       </c>
       <c r="BY4" t="n">
-        <v>-0.08115024118289597</v>
+        <v>-0.02337664209677967</v>
       </c>
       <c r="BZ4" t="n">
-        <v>-0</v>
+        <v>-0.1318044597539551</v>
       </c>
       <c r="CA4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CB4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CC4" t="n">
         <v>0</v>
@@ -2388,22 +2388,22 @@
         <v>0</v>
       </c>
       <c r="CE4" t="n">
-        <v>0.08851141071438781</v>
+        <v>-0.1021583914261066</v>
       </c>
       <c r="CF4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CG4" t="n">
-        <v>-0.09034597717424243</v>
+        <v>-0</v>
       </c>
       <c r="CH4" t="n">
-        <v>0.03555696192754586</v>
+        <v>-0.03532466201889423</v>
       </c>
       <c r="CI4" t="n">
-        <v>0</v>
+        <v>0.08458899011131685</v>
       </c>
       <c r="CJ4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CK4" t="n">
         <v>0</v>
@@ -2412,22 +2412,22 @@
         <v>0</v>
       </c>
       <c r="CM4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CN4" t="n">
-        <v>0.008902525611985226</v>
+        <v>-0.07622266115666991</v>
       </c>
       <c r="CO4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CP4" t="n">
-        <v>-0.09915967104496498</v>
+        <v>0</v>
       </c>
       <c r="CQ4" t="n">
-        <v>0.2020243685784019</v>
+        <v>0.0557340921369089</v>
       </c>
       <c r="CR4" t="n">
-        <v>0</v>
+        <v>-0.008414755707959833</v>
       </c>
       <c r="CS4" t="n">
         <v>-0</v>
@@ -2442,19 +2442,19 @@
         <v>-0</v>
       </c>
       <c r="CW4" t="n">
-        <v>0.09002061245633203</v>
+        <v>-0.07580754175083776</v>
       </c>
       <c r="CX4" t="n">
         <v>-0</v>
       </c>
       <c r="CY4" t="n">
-        <v>-0.07038525059862122</v>
+        <v>0</v>
       </c>
       <c r="CZ4" t="n">
-        <v>0.02729806942064843</v>
+        <v>-0.02465610247676257</v>
       </c>
       <c r="DA4" t="n">
-        <v>0</v>
+        <v>0.08176320215717549</v>
       </c>
       <c r="DB4" t="n">
         <v>0</v>
@@ -2463,25 +2463,25 @@
         <v>-0</v>
       </c>
       <c r="DD4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DE4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DF4" t="n">
-        <v>0.2349777769534973</v>
+        <v>-0.1214138544860826</v>
       </c>
       <c r="DG4" t="n">
         <v>-0</v>
       </c>
       <c r="DH4" t="n">
-        <v>-0.02166929037042023</v>
+        <v>-0</v>
       </c>
       <c r="DI4" t="n">
-        <v>-0.1055316206764794</v>
+        <v>0.05060995353399975</v>
       </c>
       <c r="DJ4" t="n">
-        <v>0</v>
+        <v>0.007237652848752282</v>
       </c>
       <c r="DK4" t="n">
         <v>0</v>
@@ -2490,58 +2490,58 @@
         <v>0</v>
       </c>
       <c r="DM4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DN4" t="n">
         <v>-0</v>
       </c>
       <c r="DO4" t="n">
-        <v>-0.0367631726758772</v>
+        <v>-0.04239344016925617</v>
       </c>
       <c r="DP4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DQ4" t="n">
-        <v>-0.004051192358614499</v>
+        <v>-0</v>
       </c>
       <c r="DR4" t="n">
-        <v>0.0715167290778132</v>
+        <v>0.0009569524015280327</v>
       </c>
       <c r="DS4" t="n">
-        <v>0</v>
+        <v>0.01339061053045242</v>
       </c>
       <c r="DT4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DU4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DV4" t="n">
         <v>0</v>
       </c>
       <c r="DW4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DX4" t="n">
-        <v>-0.08909740600879289</v>
+        <v>0.04107505515408476</v>
       </c>
       <c r="DY4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DZ4" t="n">
-        <v>0.07835624888962892</v>
+        <v>-0</v>
       </c>
       <c r="EA4" t="n">
-        <v>-0.0370599063272022</v>
+        <v>-0.01863605066313381</v>
       </c>
       <c r="EB4" t="n">
-        <v>0</v>
+        <v>-0.007276819296266104</v>
       </c>
       <c r="EC4" t="n">
         <v>-0</v>
       </c>
       <c r="ED4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EE4" t="n">
         <v>-0</v>
@@ -2550,46 +2550,46 @@
         <v>0</v>
       </c>
       <c r="EG4" t="n">
-        <v>0.09376187018839588</v>
+        <v>-0.04617767171618136</v>
       </c>
       <c r="EH4" t="n">
         <v>0</v>
       </c>
       <c r="EI4" t="n">
-        <v>-0.1418825015613667</v>
+        <v>0</v>
       </c>
       <c r="EJ4" t="n">
-        <v>-0.03422396121846398</v>
+        <v>-0.0003742366308802584</v>
       </c>
       <c r="EK4" t="n">
-        <v>-0</v>
+        <v>0.06937071822897516</v>
       </c>
       <c r="EL4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EM4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EN4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EO4" t="n">
         <v>0</v>
       </c>
       <c r="EP4" t="n">
-        <v>0.05536271922008922</v>
+        <v>-0.03578639701946226</v>
       </c>
       <c r="EQ4" t="n">
         <v>0</v>
       </c>
       <c r="ER4" t="n">
-        <v>0.005273636324097393</v>
+        <v>-0</v>
       </c>
       <c r="ES4" t="n">
-        <v>0.03610886591771896</v>
+        <v>-0.002511782053140976</v>
       </c>
       <c r="ET4" t="n">
-        <v>-0</v>
+        <v>0.01378986376957782</v>
       </c>
       <c r="EU4" t="n">
         <v>-0</v>
@@ -2604,49 +2604,49 @@
         <v>0</v>
       </c>
       <c r="EY4" t="n">
-        <v>0.08002202434082079</v>
+        <v>-0.07548832889363698</v>
       </c>
       <c r="EZ4" t="n">
         <v>0</v>
       </c>
       <c r="FA4" t="n">
-        <v>-0.06702033940322469</v>
+        <v>-0</v>
       </c>
       <c r="FB4" t="n">
-        <v>0.03024873203852725</v>
+        <v>-0.007989336884898357</v>
       </c>
       <c r="FC4" t="n">
-        <v>0</v>
+        <v>0.08253256689453026</v>
       </c>
       <c r="FD4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FE4" t="n">
         <v>0</v>
       </c>
       <c r="FF4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FG4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FH4" t="n">
-        <v>0.04250448936444761</v>
+        <v>-0.02667509012319998</v>
       </c>
       <c r="FI4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FJ4" t="n">
-        <v>-0.05653894632650847</v>
+        <v>-0</v>
       </c>
       <c r="FK4" t="n">
-        <v>0.007089210510830516</v>
+        <v>-0.03698981378461119</v>
       </c>
       <c r="FL4" t="n">
-        <v>0</v>
+        <v>0.1252882643213336</v>
       </c>
       <c r="FM4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FN4" t="n">
         <v>-0</v>
@@ -2655,22 +2655,22 @@
         <v>0</v>
       </c>
       <c r="FP4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FQ4" t="n">
-        <v>-0.006664874518888041</v>
+        <v>-0.003006450450050371</v>
       </c>
       <c r="FR4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FS4" t="n">
-        <v>0.05244441273605065</v>
+        <v>-0</v>
       </c>
       <c r="FT4" t="n">
-        <v>0.05328144998788379</v>
+        <v>-0.07167172005777364</v>
       </c>
       <c r="FU4" t="n">
-        <v>0</v>
+        <v>0.08244596212143086</v>
       </c>
       <c r="FV4" t="n">
         <v>-0</v>
@@ -2679,34 +2679,34 @@
         <v>-0</v>
       </c>
       <c r="FX4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FY4" t="n">
         <v>-0</v>
       </c>
       <c r="FZ4" t="n">
-        <v>0.04233191245074976</v>
+        <v>-0.04856345833787983</v>
       </c>
       <c r="GA4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="GB4" t="n">
-        <v>0.09057403785424614</v>
+        <v>-0</v>
       </c>
       <c r="GC4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="GD4" t="n">
-        <v>0</v>
+        <v>-0.09574389797521202</v>
       </c>
       <c r="GE4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="GF4" t="n">
         <v>-0</v>
       </c>
       <c r="GG4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2714,25 +2714,25 @@
         <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>-0.3215455388035593</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.1092777291766397</v>
+        <v>0.4268003676076384</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.1268308167253415</v>
+        <v>0.04173892244839422</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4935664754248817</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>-0</v>
@@ -2741,25 +2741,25 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>-0</v>
+        <v>-0.2718347124616217</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.06412432947614487</v>
+        <v>0.3772290778366779</v>
       </c>
       <c r="N5" t="n">
-        <v>-0.0396275608369712</v>
+        <v>0.1040416034487176</v>
       </c>
       <c r="O5" t="n">
         <v>-0</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.5477252231786183</v>
+        <v>-0</v>
       </c>
       <c r="R5" t="n">
         <v>-0</v>
@@ -2768,43 +2768,43 @@
         <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>-0</v>
+        <v>-0.05004081533165394</v>
       </c>
       <c r="U5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>-0.01742383525708847</v>
+        <v>0.1090151972643475</v>
       </c>
       <c r="W5" t="n">
-        <v>0.2152601892193161</v>
+        <v>0.1506715327024163</v>
       </c>
       <c r="X5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="Y5" t="n">
         <v>-0</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.2154894797148213</v>
+        <v>-0</v>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AB5" t="n">
         <v>-0</v>
       </c>
       <c r="AC5" t="n">
-        <v>0</v>
+        <v>-0.02887431776891015</v>
       </c>
       <c r="AD5" t="n">
         <v>-0</v>
       </c>
       <c r="AE5" t="n">
-        <v>-0.02102654925636835</v>
+        <v>0.03099607481832935</v>
       </c>
       <c r="AF5" t="n">
-        <v>-0.02973086897273214</v>
+        <v>-0.002171664272443816</v>
       </c>
       <c r="AG5" t="n">
         <v>-0</v>
@@ -2813,34 +2813,34 @@
         <v>0</v>
       </c>
       <c r="AI5" t="n">
-        <v>-0.0710545997298794</v>
+        <v>-0</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AK5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AL5" t="n">
-        <v>0</v>
+        <v>-0.0539421869878648</v>
       </c>
       <c r="AM5" t="n">
         <v>-0</v>
       </c>
       <c r="AN5" t="n">
-        <v>-0.009522379820394822</v>
+        <v>0.03142291941106781</v>
       </c>
       <c r="AO5" t="n">
-        <v>-0.1551025578695476</v>
+        <v>0.02255053611939785</v>
       </c>
       <c r="AP5" t="n">
         <v>-0</v>
       </c>
       <c r="AQ5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.07583028666576724</v>
+        <v>0</v>
       </c>
       <c r="AS5" t="n">
         <v>-0</v>
@@ -2849,25 +2849,25 @@
         <v>0</v>
       </c>
       <c r="AU5" t="n">
-        <v>0</v>
+        <v>-0.4019385659229635</v>
       </c>
       <c r="AV5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AW5" t="n">
-        <v>-0.1271388055309666</v>
+        <v>0.06897792228284406</v>
       </c>
       <c r="AX5" t="n">
-        <v>-0.07635608271133312</v>
+        <v>-0.1281272531239209</v>
       </c>
       <c r="AY5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AZ5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BA5" t="n">
-        <v>0.3098081293930155</v>
+        <v>0</v>
       </c>
       <c r="BB5" t="n">
         <v>-0</v>
@@ -2876,43 +2876,43 @@
         <v>-0</v>
       </c>
       <c r="BD5" t="n">
-        <v>-0</v>
+        <v>-0.02430147668617014</v>
       </c>
       <c r="BE5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BF5" t="n">
-        <v>-0.02734595515405687</v>
+        <v>0.1903385692718083</v>
       </c>
       <c r="BG5" t="n">
-        <v>-0.01906223275212978</v>
+        <v>0.2738649758045769</v>
       </c>
       <c r="BH5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BI5" t="n">
         <v>0</v>
       </c>
       <c r="BJ5" t="n">
-        <v>0.1191322764293054</v>
+        <v>-0</v>
       </c>
       <c r="BK5" t="n">
         <v>-0</v>
       </c>
       <c r="BL5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BM5" t="n">
-        <v>-0</v>
+        <v>-0.03628727823673479</v>
       </c>
       <c r="BN5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BO5" t="n">
-        <v>-0.009290804827601189</v>
+        <v>-0.001377243529933103</v>
       </c>
       <c r="BP5" t="n">
-        <v>0.001859240517111793</v>
+        <v>-0.08873255418709254</v>
       </c>
       <c r="BQ5" t="n">
         <v>0</v>
@@ -2921,160 +2921,160 @@
         <v>0</v>
       </c>
       <c r="BS5" t="n">
-        <v>-0.09126979046416837</v>
+        <v>0</v>
       </c>
       <c r="BT5" t="n">
         <v>0</v>
       </c>
       <c r="BU5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BV5" t="n">
-        <v>0</v>
+        <v>-0.2477178503924696</v>
       </c>
       <c r="BW5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BX5" t="n">
-        <v>-0.06455240822939762</v>
+        <v>0.05550396287344841</v>
       </c>
       <c r="BY5" t="n">
-        <v>-0.04359928699170577</v>
+        <v>-0.004352928206524021</v>
       </c>
       <c r="BZ5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CA5" t="n">
         <v>-0</v>
       </c>
       <c r="CB5" t="n">
-        <v>0.2796073722913304</v>
+        <v>0</v>
       </c>
       <c r="CC5" t="n">
         <v>-0</v>
       </c>
       <c r="CD5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CE5" t="n">
-        <v>-0</v>
+        <v>0.08573867346287942</v>
       </c>
       <c r="CF5" t="n">
         <v>-0</v>
       </c>
       <c r="CG5" t="n">
-        <v>0.03534254142788503</v>
+        <v>-0.09433899030873051</v>
       </c>
       <c r="CH5" t="n">
-        <v>-0.006089211357572685</v>
+        <v>0.0242901099866377</v>
       </c>
       <c r="CI5" t="n">
         <v>-0</v>
       </c>
       <c r="CJ5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CK5" t="n">
-        <v>-0.1090013767070742</v>
+        <v>-0</v>
       </c>
       <c r="CL5" t="n">
         <v>0</v>
       </c>
       <c r="CM5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CN5" t="n">
-        <v>0</v>
+        <v>-0.02291582543317137</v>
       </c>
       <c r="CO5" t="n">
         <v>-0</v>
       </c>
       <c r="CP5" t="n">
-        <v>0.016081078375334</v>
+        <v>0.04344608758541615</v>
       </c>
       <c r="CQ5" t="n">
-        <v>-0.1419910019150877</v>
+        <v>-0.0102587016080173</v>
       </c>
       <c r="CR5" t="n">
         <v>-0</v>
       </c>
       <c r="CS5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CT5" t="n">
-        <v>-0.0562216264947898</v>
+        <v>0</v>
       </c>
       <c r="CU5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CV5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CW5" t="n">
-        <v>0</v>
+        <v>0.08070271466793195</v>
       </c>
       <c r="CX5" t="n">
         <v>0</v>
       </c>
       <c r="CY5" t="n">
-        <v>0.03373216311800563</v>
+        <v>-0.09078368292945241</v>
       </c>
       <c r="CZ5" t="n">
-        <v>-0.03405599123304474</v>
+        <v>-0.007199192679304272</v>
       </c>
       <c r="DA5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DB5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DC5" t="n">
-        <v>-0.1051472370135277</v>
+        <v>0</v>
       </c>
       <c r="DD5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DE5" t="n">
         <v>0</v>
       </c>
       <c r="DF5" t="n">
-        <v>-0</v>
+        <v>0.007633889506394685</v>
       </c>
       <c r="DG5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DH5" t="n">
-        <v>0.002637325791763179</v>
+        <v>-0.04186968986327556</v>
       </c>
       <c r="DI5" t="n">
-        <v>0.01674434795444736</v>
+        <v>-0.0798733474127364</v>
       </c>
       <c r="DJ5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DK5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DL5" t="n">
-        <v>0.0002177650008323897</v>
+        <v>-0</v>
       </c>
       <c r="DM5" t="n">
         <v>-0</v>
       </c>
       <c r="DN5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DO5" t="n">
-        <v>-0</v>
+        <v>0.06040769406593899</v>
       </c>
       <c r="DP5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DQ5" t="n">
-        <v>-0.04697383563331691</v>
+        <v>-0.1282058627817134</v>
       </c>
       <c r="DR5" t="n">
-        <v>-0.02348334876399173</v>
+        <v>0.003082269080396409</v>
       </c>
       <c r="DS5" t="n">
         <v>-0</v>
@@ -3083,7 +3083,7 @@
         <v>-0</v>
       </c>
       <c r="DU5" t="n">
-        <v>-0.02929837510303617</v>
+        <v>0</v>
       </c>
       <c r="DV5" t="n">
         <v>-0</v>
@@ -3092,25 +3092,25 @@
         <v>-0</v>
       </c>
       <c r="DX5" t="n">
-        <v>0</v>
+        <v>-0.01187928681479571</v>
       </c>
       <c r="DY5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DZ5" t="n">
-        <v>-0.006316429075153166</v>
+        <v>0.007776695515561097</v>
       </c>
       <c r="EA5" t="n">
-        <v>0.03853685714806768</v>
+        <v>0.01436470848984942</v>
       </c>
       <c r="EB5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EC5" t="n">
         <v>0</v>
       </c>
       <c r="ED5" t="n">
-        <v>-0.0792945134749722</v>
+        <v>0</v>
       </c>
       <c r="EE5" t="n">
         <v>-0</v>
@@ -3119,25 +3119,25 @@
         <v>-0</v>
       </c>
       <c r="EG5" t="n">
-        <v>0</v>
+        <v>0.008623267379450121</v>
       </c>
       <c r="EH5" t="n">
         <v>-0</v>
       </c>
       <c r="EI5" t="n">
-        <v>0.0954178631992411</v>
+        <v>-0.03287586678445679</v>
       </c>
       <c r="EJ5" t="n">
-        <v>0.06418194619269067</v>
+        <v>-0.02019692815802627</v>
       </c>
       <c r="EK5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EL5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EM5" t="n">
-        <v>-0.1424507367165128</v>
+        <v>0</v>
       </c>
       <c r="EN5" t="n">
         <v>0</v>
@@ -3146,136 +3146,136 @@
         <v>-0</v>
       </c>
       <c r="EP5" t="n">
-        <v>-0</v>
+        <v>0.08328260824759384</v>
       </c>
       <c r="EQ5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="ER5" t="n">
-        <v>0.02487195800783166</v>
+        <v>-0.06429325396644589</v>
       </c>
       <c r="ES5" t="n">
-        <v>-0.06830944475847206</v>
+        <v>0.06278479355845612</v>
       </c>
       <c r="ET5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EU5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EV5" t="n">
-        <v>0.09409933473423752</v>
+        <v>-0</v>
       </c>
       <c r="EW5" t="n">
         <v>0</v>
       </c>
       <c r="EX5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EY5" t="n">
-        <v>-0</v>
+        <v>0.08903957109298768</v>
       </c>
       <c r="EZ5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FA5" t="n">
-        <v>0.04042102083080933</v>
+        <v>-0.09463752330257852</v>
       </c>
       <c r="FB5" t="n">
-        <v>-0.0140521624973776</v>
+        <v>0.01800727865349654</v>
       </c>
       <c r="FC5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FD5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FE5" t="n">
-        <v>-0.1095106790398117</v>
+        <v>-0</v>
       </c>
       <c r="FF5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FG5" t="n">
         <v>0</v>
       </c>
       <c r="FH5" t="n">
-        <v>-0</v>
+        <v>0.0414521633608991</v>
       </c>
       <c r="FI5" t="n">
         <v>-0</v>
       </c>
       <c r="FJ5" t="n">
-        <v>0.05447269324616513</v>
+        <v>0.04354840130687807</v>
       </c>
       <c r="FK5" t="n">
-        <v>0.02329883529412076</v>
+        <v>-0.03291359847804542</v>
       </c>
       <c r="FL5" t="n">
         <v>0</v>
       </c>
       <c r="FM5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FN5" t="n">
-        <v>0.07828483114627088</v>
+        <v>-0</v>
       </c>
       <c r="FO5" t="n">
         <v>0</v>
       </c>
       <c r="FP5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FQ5" t="n">
-        <v>0</v>
+        <v>-0.01221464163930013</v>
       </c>
       <c r="FR5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FS5" t="n">
-        <v>-0.002018901999313671</v>
+        <v>0.02831107797667131</v>
       </c>
       <c r="FT5" t="n">
-        <v>-0.03466274638096026</v>
+        <v>-0.01839111089489138</v>
       </c>
       <c r="FU5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FV5" t="n">
         <v>0</v>
       </c>
       <c r="FW5" t="n">
-        <v>-0.1316883068261281</v>
+        <v>-0</v>
       </c>
       <c r="FX5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FY5" t="n">
         <v>0</v>
       </c>
       <c r="FZ5" t="n">
-        <v>0</v>
+        <v>0.06933134074777453</v>
       </c>
       <c r="GA5" t="n">
         <v>0</v>
       </c>
       <c r="GB5" t="n">
-        <v>-0.0002215206853716623</v>
+        <v>0.06106598869935288</v>
       </c>
       <c r="GC5" t="n">
         <v>-0</v>
       </c>
       <c r="GD5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="GE5" t="n">
         <v>0</v>
       </c>
       <c r="GF5" t="n">
-        <v>-0.01778319799619772</v>
+        <v>0</v>
       </c>
       <c r="GG5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -3283,214 +3283,214 @@
         <v>0</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>-0.4984606456358585</v>
       </c>
       <c r="C6" t="n">
         <v>-0</v>
       </c>
       <c r="D6" t="n">
-        <v>-0</v>
+        <v>0.1630556590172297</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.03995414855452727</v>
+        <v>0.1726498722410141</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3633237534520066</v>
+        <v>-0</v>
       </c>
       <c r="G6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.1506643917065269</v>
+        <v>-0</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>-0.3279555481603417</v>
       </c>
       <c r="L6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>-0</v>
+        <v>0.1702610439958268</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.04882783749511052</v>
+        <v>0.09870378554691323</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3002592867203225</v>
+        <v>-0</v>
       </c>
       <c r="P6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.114069404388243</v>
+        <v>-0</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>-0</v>
+        <v>-0.04977107854097373</v>
       </c>
       <c r="U6" t="n">
         <v>-0</v>
       </c>
       <c r="V6" t="n">
-        <v>0</v>
+        <v>0.07105694791705165</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.06201867568194852</v>
+        <v>0.1314246000310552</v>
       </c>
       <c r="X6" t="n">
-        <v>0.0804818223658729</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.009367245902887397</v>
+        <v>-0</v>
       </c>
       <c r="AA6" t="n">
         <v>-0</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0</v>
+        <v>-0.008674013499658548</v>
       </c>
       <c r="AD6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0</v>
+        <v>0.1101794412399949</v>
       </c>
       <c r="AF6" t="n">
-        <v>-0.0821893655759694</v>
+        <v>0.02797574269990794</v>
       </c>
       <c r="AG6" t="n">
-        <v>-0.01821382165463582</v>
+        <v>0</v>
       </c>
       <c r="AH6" t="n">
         <v>-0</v>
       </c>
       <c r="AI6" t="n">
-        <v>-0.0378948236994763</v>
+        <v>-0</v>
       </c>
       <c r="AJ6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AK6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AL6" t="n">
-        <v>-0</v>
+        <v>-0.06945021309965831</v>
       </c>
       <c r="AM6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AN6" t="n">
-        <v>0</v>
+        <v>0.01504631513886189</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.02565533786305056</v>
+        <v>0.08275532588214642</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.05255170457249865</v>
+        <v>-0</v>
       </c>
       <c r="AQ6" t="n">
         <v>-0</v>
       </c>
       <c r="AR6" t="n">
-        <v>0.005724092566375518</v>
+        <v>-0</v>
       </c>
       <c r="AS6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AT6" t="n">
         <v>0</v>
       </c>
       <c r="AU6" t="n">
-        <v>0</v>
+        <v>-0.2217662334140048</v>
       </c>
       <c r="AV6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AW6" t="n">
-        <v>0</v>
+        <v>0.09189041611866648</v>
       </c>
       <c r="AX6" t="n">
-        <v>-0.1010338017301438</v>
+        <v>0.1593328705998186</v>
       </c>
       <c r="AY6" t="n">
-        <v>0.1589597129313061</v>
+        <v>-0</v>
       </c>
       <c r="AZ6" t="n">
         <v>-0</v>
       </c>
       <c r="BA6" t="n">
-        <v>-0.0647297863061178</v>
+        <v>-0</v>
       </c>
       <c r="BB6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BC6" t="n">
         <v>-0</v>
       </c>
       <c r="BD6" t="n">
-        <v>-0</v>
+        <v>-0.1701912849948955</v>
       </c>
       <c r="BE6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BF6" t="n">
-        <v>-0</v>
+        <v>0.1496924177117338</v>
       </c>
       <c r="BG6" t="n">
-        <v>-0.03168809991159487</v>
+        <v>0.1637932605620342</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.0667738043559388</v>
+        <v>-0</v>
       </c>
       <c r="BI6" t="n">
         <v>-0</v>
       </c>
       <c r="BJ6" t="n">
-        <v>-0.1083331354400666</v>
+        <v>0</v>
       </c>
       <c r="BK6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BL6" t="n">
         <v>-0</v>
       </c>
       <c r="BM6" t="n">
-        <v>-0</v>
+        <v>-0.01750633267065132</v>
       </c>
       <c r="BN6" t="n">
         <v>0</v>
       </c>
       <c r="BO6" t="n">
-        <v>0</v>
+        <v>0.02805024861406306</v>
       </c>
       <c r="BP6" t="n">
-        <v>-0.01593945027377974</v>
+        <v>-0.0150707712974798</v>
       </c>
       <c r="BQ6" t="n">
-        <v>-0.03336987623681225</v>
+        <v>0</v>
       </c>
       <c r="BR6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BS6" t="n">
-        <v>-0.02574533859025392</v>
+        <v>0</v>
       </c>
       <c r="BT6" t="n">
         <v>0</v>
@@ -3499,214 +3499,214 @@
         <v>0</v>
       </c>
       <c r="BV6" t="n">
-        <v>-0</v>
+        <v>-0.1869627900357449</v>
       </c>
       <c r="BW6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BX6" t="n">
-        <v>0</v>
+        <v>0.08269522822173711</v>
       </c>
       <c r="BY6" t="n">
-        <v>-0.03899192109807578</v>
+        <v>0.07160141034564049</v>
       </c>
       <c r="BZ6" t="n">
-        <v>0.1174455046826923</v>
+        <v>-0</v>
       </c>
       <c r="CA6" t="n">
         <v>0</v>
       </c>
       <c r="CB6" t="n">
-        <v>-0.05104605489494454</v>
+        <v>-0</v>
       </c>
       <c r="CC6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CD6" t="n">
         <v>-0</v>
       </c>
       <c r="CE6" t="n">
-        <v>-0</v>
+        <v>0.07314132801364766</v>
       </c>
       <c r="CF6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CG6" t="n">
-        <v>0</v>
+        <v>-0.04829610327900825</v>
       </c>
       <c r="CH6" t="n">
-        <v>0.01642348486253143</v>
+        <v>0.0220016211943641</v>
       </c>
       <c r="CI6" t="n">
-        <v>-0.05485353057649208</v>
+        <v>0</v>
       </c>
       <c r="CJ6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CK6" t="n">
-        <v>0.03227814169075361</v>
+        <v>-0</v>
       </c>
       <c r="CL6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CM6" t="n">
         <v>-0</v>
       </c>
       <c r="CN6" t="n">
-        <v>0</v>
+        <v>-0.07464434621248818</v>
       </c>
       <c r="CO6" t="n">
         <v>0</v>
       </c>
       <c r="CP6" t="n">
-        <v>0</v>
+        <v>-0.1890121403656911</v>
       </c>
       <c r="CQ6" t="n">
-        <v>0.107089645675316</v>
+        <v>-0.0002884619474195425</v>
       </c>
       <c r="CR6" t="n">
-        <v>0.063428800104674</v>
+        <v>-0</v>
       </c>
       <c r="CS6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CT6" t="n">
-        <v>-0.004134201112238744</v>
+        <v>-0</v>
       </c>
       <c r="CU6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CV6" t="n">
         <v>0</v>
       </c>
       <c r="CW6" t="n">
-        <v>0</v>
+        <v>0.08217006691740611</v>
       </c>
       <c r="CX6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CY6" t="n">
-        <v>-0</v>
+        <v>-0.03760318759258864</v>
       </c>
       <c r="CZ6" t="n">
-        <v>0.01769971092992787</v>
+        <v>0.006921899711900212</v>
       </c>
       <c r="DA6" t="n">
-        <v>-0.05419189384056852</v>
+        <v>-0</v>
       </c>
       <c r="DB6" t="n">
         <v>-0</v>
       </c>
       <c r="DC6" t="n">
-        <v>0.04716371191490735</v>
+        <v>0</v>
       </c>
       <c r="DD6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DE6" t="n">
         <v>-0</v>
       </c>
       <c r="DF6" t="n">
-        <v>0</v>
+        <v>0.1409288196047623</v>
       </c>
       <c r="DG6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DH6" t="n">
-        <v>0</v>
+        <v>-0.06822517556188347</v>
       </c>
       <c r="DI6" t="n">
-        <v>0.0105100647457428</v>
+        <v>-0.005384569511356482</v>
       </c>
       <c r="DJ6" t="n">
-        <v>-0.01848907107078376</v>
+        <v>0</v>
       </c>
       <c r="DK6" t="n">
         <v>0</v>
       </c>
       <c r="DL6" t="n">
-        <v>0.001674231217383451</v>
+        <v>-0</v>
       </c>
       <c r="DM6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DN6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DO6" t="n">
-        <v>0</v>
+        <v>0.007838807386637002</v>
       </c>
       <c r="DP6" t="n">
         <v>0</v>
       </c>
       <c r="DQ6" t="n">
-        <v>0</v>
+        <v>-0.022049683320956</v>
       </c>
       <c r="DR6" t="n">
-        <v>0.03242795979754133</v>
+        <v>-0.04447367122941184</v>
       </c>
       <c r="DS6" t="n">
-        <v>0.008638746898398227</v>
+        <v>-0</v>
       </c>
       <c r="DT6" t="n">
         <v>0</v>
       </c>
       <c r="DU6" t="n">
-        <v>0.02509718468816059</v>
+        <v>0</v>
       </c>
       <c r="DV6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DW6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="DX6" t="n">
-        <v>-0</v>
+        <v>0.1093686026545412</v>
       </c>
       <c r="DY6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="DZ6" t="n">
-        <v>-0</v>
+        <v>-0.0463918430016036</v>
       </c>
       <c r="EA6" t="n">
-        <v>-0.01756345256323576</v>
+        <v>0.00413492236823502</v>
       </c>
       <c r="EB6" t="n">
-        <v>0.01148552363879394</v>
+        <v>-0</v>
       </c>
       <c r="EC6" t="n">
         <v>0</v>
       </c>
       <c r="ED6" t="n">
-        <v>0.0006434037135807334</v>
+        <v>-0</v>
       </c>
       <c r="EE6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EF6" t="n">
         <v>-0</v>
       </c>
       <c r="EG6" t="n">
-        <v>-0</v>
+        <v>0.05744850113713924</v>
       </c>
       <c r="EH6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EI6" t="n">
-        <v>0</v>
+        <v>0.05538835150769398</v>
       </c>
       <c r="EJ6" t="n">
-        <v>-0.04273664967317432</v>
+        <v>0.06456316018268303</v>
       </c>
       <c r="EK6" t="n">
-        <v>-0.0516234108503514</v>
+        <v>0</v>
       </c>
       <c r="EL6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="EM6" t="n">
-        <v>0.01394517879277145</v>
+        <v>0</v>
       </c>
       <c r="EN6" t="n">
         <v>0</v>
@@ -3715,25 +3715,25 @@
         <v>0</v>
       </c>
       <c r="EP6" t="n">
-        <v>-0</v>
+        <v>0.02534774737078672</v>
       </c>
       <c r="EQ6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="ER6" t="n">
-        <v>0</v>
+        <v>-0.05251768604493646</v>
       </c>
       <c r="ES6" t="n">
-        <v>0.05688643568047742</v>
+        <v>-0.002826237861208346</v>
       </c>
       <c r="ET6" t="n">
-        <v>-0.04117664096080323</v>
+        <v>0</v>
       </c>
       <c r="EU6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="EV6" t="n">
-        <v>0.02594048006618603</v>
+        <v>-0</v>
       </c>
       <c r="EW6" t="n">
         <v>0</v>
@@ -3742,106 +3742,106 @@
         <v>-0</v>
       </c>
       <c r="EY6" t="n">
-        <v>-0</v>
+        <v>0.08255266764086829</v>
       </c>
       <c r="EZ6" t="n">
         <v>0</v>
       </c>
       <c r="FA6" t="n">
-        <v>0</v>
+        <v>-0.02979239188072513</v>
       </c>
       <c r="FB6" t="n">
-        <v>0.01976173765726176</v>
+        <v>0.02332877836078678</v>
       </c>
       <c r="FC6" t="n">
-        <v>-0.05401728632134003</v>
+        <v>0</v>
       </c>
       <c r="FD6" t="n">
         <v>0</v>
       </c>
       <c r="FE6" t="n">
-        <v>0.04723121077414497</v>
+        <v>-0</v>
       </c>
       <c r="FF6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FG6" t="n">
         <v>-0</v>
       </c>
       <c r="FH6" t="n">
-        <v>-0</v>
+        <v>-0.04531463150076858</v>
       </c>
       <c r="FI6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FJ6" t="n">
-        <v>0</v>
+        <v>0.04543308323280197</v>
       </c>
       <c r="FK6" t="n">
-        <v>-0.02588245055728845</v>
+        <v>-0.0177003039992163</v>
       </c>
       <c r="FL6" t="n">
-        <v>0.06440261606556646</v>
+        <v>0</v>
       </c>
       <c r="FM6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FN6" t="n">
-        <v>-0.05252365315753169</v>
+        <v>0</v>
       </c>
       <c r="FO6" t="n">
         <v>-0</v>
       </c>
       <c r="FP6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FQ6" t="n">
-        <v>-0</v>
+        <v>0.1238616740461258</v>
       </c>
       <c r="FR6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="FS6" t="n">
-        <v>0</v>
+        <v>-0.08138835912372706</v>
       </c>
       <c r="FT6" t="n">
-        <v>0.04750893534897364</v>
+        <v>-0.1981051395525977</v>
       </c>
       <c r="FU6" t="n">
-        <v>-0.06063462969960533</v>
+        <v>0</v>
       </c>
       <c r="FV6" t="n">
         <v>-0</v>
       </c>
       <c r="FW6" t="n">
-        <v>0.06203606566416139</v>
+        <v>0</v>
       </c>
       <c r="FX6" t="n">
         <v>-0</v>
       </c>
       <c r="FY6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="FZ6" t="n">
-        <v>0</v>
+        <v>-0.008877747759138481</v>
       </c>
       <c r="GA6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="GB6" t="n">
-        <v>-0</v>
+        <v>0.01675310711426355</v>
       </c>
       <c r="GC6" t="n">
         <v>-0</v>
       </c>
       <c r="GD6" t="n">
-        <v>0.07730740638112882</v>
+        <v>0</v>
       </c>
       <c r="GE6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="GF6" t="n">
-        <v>-0.004539207090892953</v>
+        <v>-0</v>
       </c>
       <c r="GG6" t="n">
         <v>-0</v>

</xml_diff>